<commit_message>
- fixed tests and added two new testdata - Tests cover now a bigger range of cases
</commit_message>
<xml_diff>
--- a/Testing/TestData/test_data_types.xlsx
+++ b/Testing/TestData/test_data_types.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZbwTechniker\6tSemester\Diplom Abschlussarbeit\Entwicklung\Offerten Automatisierung\TestForExcelEditor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZbwTechniker\6tSemester\Diplom Abschlussarbeit\Entwicklung\Realisierung\Offerten-Automatisierung\Offerten-Automatisierung\Testing\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7D3BBA-0158-4BDE-912C-3D39F2B63959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A79094-5390-4957-B9AD-9E8DA535D2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="2700" windowWidth="28800" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="CurrencyValue1">Tabelle1!$M$23</definedName>
+    <definedName name="NumberValue1">Tabelle1!$A$1</definedName>
+    <definedName name="StringValue1">Tabelle1!$I$16</definedName>
+    <definedName name="StringValue2">Tabelle1!$D$27</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,21 +31,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Press</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Round</t>
   </si>
   <si>
-    <t>Parallel</t>
+    <t>Word.#.Exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$CHF]"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -354,29 +361,32 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1">
+        <v>2311313</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M23">
+      <c r="M23" s="1">
         <v>50000</v>
       </c>
     </row>
     <row r="27" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>